<commit_message>
Pasar divisor a constantes y leer propiedades de Header de archivo
</commit_message>
<xml_diff>
--- a/code/output.xlsx
+++ b/code/output.xlsx
@@ -15,10 +15,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
-    <t>Out Col 7</t>
+    <t>Output7</t>
   </si>
   <si>
-    <t>Out Col 1</t>
+    <t>Output1</t>
   </si>
   <si>
     <t>John</t>
@@ -89,8 +89,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.42578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.42578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.42578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Declarar ifs para checar indice de los headers
</commit_message>
<xml_diff>
--- a/code/output.xlsx
+++ b/code/output.xlsx
@@ -13,12 +13,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Output7</t>
   </si>
   <si>
     <t>Output1</t>
+  </si>
+  <si>
+    <t>Output2</t>
   </si>
   <si>
     <t>John</t>
@@ -90,63 +93,85 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.42578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.42578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.42578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
+      <c r="C4" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambiar indices si no coinciden con nombre de la columna
</commit_message>
<xml_diff>
--- a/code/output.xlsx
+++ b/code/output.xlsx
@@ -13,21 +13,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
-  <si>
-    <t>Output7</t>
-  </si>
-  <si>
-    <t>Output1</t>
-  </si>
-  <si>
-    <t>Output2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+  <si>
+    <t>Output_7</t>
+  </si>
+  <si>
+    <t>Output_1</t>
+  </si>
+  <si>
+    <t>Output_2</t>
   </si>
   <si>
     <t>John</t>
   </si>
   <si>
     <t>Josh</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>Viridian</t>
@@ -94,7 +97,8 @@
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.42578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.42578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.42578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="9.42578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -107,6 +111,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -118,32 +125,41 @@
       <c r="C2" t="n">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
         <v>43</v>
       </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -151,16 +167,22 @@
       <c r="C5" t="n">
         <v>48</v>
       </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
         <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -168,10 +190,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imprimir datos estaticos a Excel
</commit_message>
<xml_diff>
--- a/code/output.xlsx
+++ b/code/output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Output_7</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Josh</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
   <si>
     <t>Viridian</t>
@@ -125,41 +122,41 @@
       <c r="C2" t="n">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
+      <c r="D3" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="D4" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -167,22 +164,22 @@
       <c r="C5" t="n">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
+      <c r="D5" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
+      <c r="D6" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -190,13 +187,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="D7" t="n">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imprimir formulas basicas a Excel
</commit_message>
<xml_diff>
--- a/code/output.xlsx
+++ b/code/output.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Output_7</t>
   </si>
@@ -96,6 +96,7 @@
     <col min="2" max="2" width="9.42578125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.42578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.42578125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="9.42578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -111,6 +112,9 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -125,6 +129,9 @@
       <c r="D2" t="n">
         <v>6.0</v>
       </c>
+      <c r="E2">
+        <f>SUM(C2:C7)</f>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -139,6 +146,9 @@
       <c r="D3" t="n">
         <v>6.0</v>
       </c>
+      <c r="E3">
+        <f>SUM(C2:C7)</f>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -152,6 +162,9 @@
       </c>
       <c r="D4" t="n">
         <v>6.0</v>
+      </c>
+      <c r="E4">
+        <f>SUM(C2:C7)</f>
       </c>
     </row>
     <row r="5">
@@ -167,6 +180,9 @@
       <c r="D5" t="n">
         <v>6.0</v>
       </c>
+      <c r="E5">
+        <f>SUM(C2:C7)</f>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -181,6 +197,9 @@
       <c r="D6" t="n">
         <v>6.0</v>
       </c>
+      <c r="E6">
+        <f>SUM(C2:C7)</f>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -194,6 +213,9 @@
       </c>
       <c r="D7" t="n">
         <v>6.0</v>
+      </c>
+      <c r="E7">
+        <f>SUM(C2:C7)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>